<commit_message>
Metadata Update - ReadMe
& shp file attributes.
+ Excel Site Description w/ Table 6 with spp abbreviations
</commit_message>
<xml_diff>
--- a/Spatial_data/UVic/Harrop-Archibald 2008/Site Descriptions 2008/Site Descriptions 2008 Metadata.xlsx
+++ b/Spatial_data/UVic/Harrop-Archibald 2008/Site Descriptions 2008/Site Descriptions 2008 Metadata.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Documents\GitHub\Github Shackelford-lab\Shackelford-lab\Spatial_data\UVic\Harrop-Archibald 2008\Site Descriptions 2007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Documents\GitHub\Github Shackelford-lab\Shackelford-lab\Spatial_data\UVic\Harrop-Archibald 2008\Site Descriptions 2008\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D10CEF-9897-4E15-9B26-5D6A91DB5E7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699622A8-618B-40F4-A8EA-027CCC0CAE8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="2385" windowWidth="17400" windowHeight="10785" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
+    <workbookView xWindow="12780" yWindow="1620" windowWidth="12210" windowHeight="14595" activeTab="1" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
+    <sheet name="Species Abbreviations" sheetId="5" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Species Abbreviations'!$B$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="420">
   <si>
     <t>Data table metadata</t>
   </si>
@@ -247,6 +251,1056 @@
     <t xml:space="preserve">Percent# Attributes: the percentaage of the most abundant plant after 'SubSpecies'. 
 E.g. Percent1, Percent2, Percent3…
 </t>
+  </si>
+  <si>
+    <t>QG</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Cspp</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>RPU</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to 'Species Abbreviations' on the other Excel Sheet. </t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>SAU</t>
+  </si>
+  <si>
+    <t>Shrub</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Cotoneaster sp</t>
+  </si>
+  <si>
+    <t>COspp</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>PMY</t>
+  </si>
+  <si>
+    <t>SDO</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>AFF</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>SRP</t>
+  </si>
+  <si>
+    <t>RSA</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Rhododendron</t>
+  </si>
+  <si>
+    <t>Rspp</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>RV</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>PMU</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>RDI</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>EHE</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>TOF</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>PMA</t>
+  </si>
+  <si>
+    <t>Common Vetch Vicia sativa</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>SCO</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>Creeping buttercup Ranunculus repens</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>Cyclamen spp</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>LAN</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>EW</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
+  <si>
+    <t>CSII</t>
+  </si>
+  <si>
+    <t>UD</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>ROC</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>SSY</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Common name</t>
+  </si>
+  <si>
+    <t>Arbutus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arbutus menziesii</t>
+  </si>
+  <si>
+    <t>Nutrient ISG #</t>
+  </si>
+  <si>
+    <t>Moisture ISG #</t>
+  </si>
+  <si>
+    <t>Bigleaf Maple</t>
+  </si>
+  <si>
+    <t>Acer macrophyllum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitter Cherry </t>
+  </si>
+  <si>
+    <t>Prunus emarginata</t>
+  </si>
+  <si>
+    <t>Populus balsamifera ssp. Trichocarpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Cottonwood </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Hawthorn </t>
+  </si>
+  <si>
+    <t>Crataegus douglasii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cascara </t>
+  </si>
+  <si>
+    <t>Rhamnus purshiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chestnut </t>
+  </si>
+  <si>
+    <t>Castanea sp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Douglas-Fir </t>
+  </si>
+  <si>
+    <t>Pseudotsuga menziesii ssp. Menziesii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English Hawthorn </t>
+  </si>
+  <si>
+    <t>Crataegus monogyna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garry Oak </t>
+  </si>
+  <si>
+    <t>Quercus garryana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Fir </t>
+  </si>
+  <si>
+    <t>Abies grandis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Crab Apple </t>
+  </si>
+  <si>
+    <t>Malus fusca</t>
+  </si>
+  <si>
+    <t>Physocarpus capitatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Ninebark </t>
+  </si>
+  <si>
+    <t>Pacific Willow</t>
+  </si>
+  <si>
+    <t>Salix lucida ssp. Lasiandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Yew </t>
+  </si>
+  <si>
+    <t>Taxus brevifolia</t>
+  </si>
+  <si>
+    <t>Red Alder</t>
+  </si>
+  <si>
+    <t>Alnus rubra</t>
+  </si>
+  <si>
+    <t>Rowan Tree</t>
+  </si>
+  <si>
+    <t>Sorbus aucuparia</t>
+  </si>
+  <si>
+    <t>Salix scouleriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scouler’s Willow </t>
+  </si>
+  <si>
+    <t>Sitka Willow</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Salix sitchensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trembling Aspen </t>
+  </si>
+  <si>
+    <t>Populus tremuloides</t>
+  </si>
+  <si>
+    <t>Western Hemlock</t>
+  </si>
+  <si>
+    <t>Tsuga heterophylla</t>
+  </si>
+  <si>
+    <t>Thuja plicata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Redcedar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baldhip Rose </t>
+  </si>
+  <si>
+    <t>Rosa gymnocarpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Twinberry </t>
+  </si>
+  <si>
+    <t>Lonicera involucrata</t>
+  </si>
+  <si>
+    <t>Common Periwinkle</t>
+  </si>
+  <si>
+    <t>Vinca minor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Snowberry </t>
+  </si>
+  <si>
+    <t>Symphoricarpos albus</t>
+  </si>
+  <si>
+    <t>Cotoneaster</t>
+  </si>
+  <si>
+    <t>Daphne</t>
+  </si>
+  <si>
+    <t>Daphne laureola</t>
+  </si>
+  <si>
+    <t>Deer Fern</t>
+  </si>
+  <si>
+    <t>Blechnum spicant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dull Oregon Grape </t>
+  </si>
+  <si>
+    <t>Mahonia nervosa</t>
+  </si>
+  <si>
+    <t>English Holly</t>
+  </si>
+  <si>
+    <t>Ilex aquifolium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English Ivy </t>
+  </si>
+  <si>
+    <t>Hedera helix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falsebox </t>
+  </si>
+  <si>
+    <t>Paxistima myrsinites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardhack </t>
+  </si>
+  <si>
+    <t>Spiraea douglasii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himalayan Blackberry </t>
+  </si>
+  <si>
+    <t>Rubus discolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian plum </t>
+  </si>
+  <si>
+    <t>Oemleria cerasiformis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lady Fern </t>
+  </si>
+  <si>
+    <t>Athyrium filix-femina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licorice Fern </t>
+  </si>
+  <si>
+    <t>Polypodium glycyrrhiza</t>
+  </si>
+  <si>
+    <t>Mock-Orange</t>
+  </si>
+  <si>
+    <t>Philadelphus lewisii</t>
+  </si>
+  <si>
+    <t>Morning Glory</t>
+  </si>
+  <si>
+    <t>Convolvulus arvensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nootka Rose </t>
+  </si>
+  <si>
+    <t>Rosa nutkana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oceanspray </t>
+  </si>
+  <si>
+    <t>Holodiscus discolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Elderberry </t>
+  </si>
+  <si>
+    <t>Sambucus racemosa ssp. Pubens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Flowering Current </t>
+  </si>
+  <si>
+    <t>Ribes sanguineum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Huckleberry </t>
+  </si>
+  <si>
+    <t>Vaccinium parvifolium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red-osier Dogwood </t>
+  </si>
+  <si>
+    <t>Cornus stolonifera</t>
+  </si>
+  <si>
+    <t>Rhododendron spp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salal </t>
+  </si>
+  <si>
+    <t>Gaultheria shallon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonberry </t>
+  </si>
+  <si>
+    <t>Rubus spectabilis</t>
+  </si>
+  <si>
+    <t>Saskatoon</t>
+  </si>
+  <si>
+    <t>Amelanchier alnifolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scotch broom </t>
+  </si>
+  <si>
+    <t>Cytisus scoparius</t>
+  </si>
+  <si>
+    <t>Invasive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sticky Current </t>
+  </si>
+  <si>
+    <t>Ribes viscosissimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. John’s-wort </t>
+  </si>
+  <si>
+    <t>Hypericum formosum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sword Fern </t>
+  </si>
+  <si>
+    <t>Polystichum munitum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tall Oregon grape </t>
+  </si>
+  <si>
+    <t>Mahonia aquifolium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thimbleberry </t>
+  </si>
+  <si>
+    <t>Rubus parviflorus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trailing Blackberry </t>
+  </si>
+  <si>
+    <t>Rubus ursinus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Trumpet Honeysuckle </t>
+  </si>
+  <si>
+    <t>Lonicera ciliosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Gooseberry </t>
+  </si>
+  <si>
+    <t>Ribes divaricatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baneberry </t>
+  </si>
+  <si>
+    <t>Actaea rubra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big-Leaved Sandwort </t>
+  </si>
+  <si>
+    <t>Moehringia macrophylla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Nightshade </t>
+  </si>
+  <si>
+    <t>Solanum dulcamara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bracken Fern </t>
+  </si>
+  <si>
+    <t>Pteridium aquilinum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broad Leaved Helleborine </t>
+  </si>
+  <si>
+    <t>Epipactis helleborine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broad Leaved Star Flower </t>
+  </si>
+  <si>
+    <t>Trientalis latifolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada Thistle </t>
+  </si>
+  <si>
+    <t>Cirsium arvense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada Violet </t>
+  </si>
+  <si>
+    <t>Viola canadensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaver </t>
+  </si>
+  <si>
+    <t>Galium aparine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Dandelion </t>
+  </si>
+  <si>
+    <t>Taraxacum officinale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Horsetail </t>
+  </si>
+  <si>
+    <t>Equisetum arvense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Plantain </t>
+  </si>
+  <si>
+    <t>Plantago major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooley’s Hedge Nettle </t>
+  </si>
+  <si>
+    <t>Stachys cooleyae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cutleaf Geranium </t>
+  </si>
+  <si>
+    <t>Geranium dissectum L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclamen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">English Daisy </t>
+  </si>
+  <si>
+    <t>Bellis perennis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Lily-Of-The-Valley </t>
+  </si>
+  <si>
+    <t>Maianthemum dilatatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Few-Seeded Bitter-Cress </t>
+  </si>
+  <si>
+    <t>Cardamine oligosperma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig Buttercup </t>
+  </si>
+  <si>
+    <t>Ranunculus ficaria</t>
+  </si>
+  <si>
+    <t>Foamflower</t>
+  </si>
+  <si>
+    <t>Tiarella trifoliata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fringecup </t>
+  </si>
+  <si>
+    <t>Tellima grandiflora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedge Mustard </t>
+  </si>
+  <si>
+    <t>Sisymbrium officinale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herb-Robert </t>
+  </si>
+  <si>
+    <t>Geranium robertianum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kneeling Angelica </t>
+  </si>
+  <si>
+    <t>Angelica genuflexa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamium </t>
+  </si>
+  <si>
+    <t>Lamiaceae spp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-Leaved Avens </t>
+  </si>
+  <si>
+    <t>Geum macrophyllum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lyre-Leaved Rockcress </t>
+  </si>
+  <si>
+    <t>Arabis lyrata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexican Hedge Nettle </t>
+  </si>
+  <si>
+    <t>Stachys mexicana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miner’s Lettuce </t>
+  </si>
+  <si>
+    <t>Claytonia perfoliata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Money Plant </t>
+  </si>
+  <si>
+    <t>Lunaria annua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountain Sweet-Cicely </t>
+  </si>
+  <si>
+    <t>Osmorhiza chilensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nipplewort </t>
+  </si>
+  <si>
+    <t>Lapsana communis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Sanicle </t>
+  </si>
+  <si>
+    <t>Sanicula crassicaulis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Water-Parsley </t>
+  </si>
+  <si>
+    <t>Oenanthe sarmentosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathfinder </t>
+  </si>
+  <si>
+    <t>Adenocaulon bicolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poison-Hemlock </t>
+  </si>
+  <si>
+    <t>Conium maculatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purple-Leaved Willowherb </t>
+  </si>
+  <si>
+    <t>Epilobium watsonii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purple Peavine </t>
+  </si>
+  <si>
+    <t>Lathyrus nevadensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scouler’s Harebell </t>
+  </si>
+  <si>
+    <t>Campanula scouleri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scouring-Rush </t>
+  </si>
+  <si>
+    <t>Equisetum hyemale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siberian Miner’s-Lettuce </t>
+  </si>
+  <si>
+    <t>Claytonia sibirica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitka Sedge </t>
+  </si>
+  <si>
+    <t>Carex sitchensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skunk Cabbage </t>
+  </si>
+  <si>
+    <t>Lysichitum americanum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stinging Nettle </t>
+  </si>
+  <si>
+    <t>Urtica dioica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweet-Scented Bedstraw </t>
+  </si>
+  <si>
+    <t>Galium trilorum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanilla-Leaf </t>
+  </si>
+  <si>
+    <t>Achlys triphylla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wall Lettuce </t>
+  </si>
+  <si>
+    <t>Lactuca muralis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Buttercup </t>
+  </si>
+  <si>
+    <t>Ranunculus occidentalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Dock </t>
+  </si>
+  <si>
+    <t>Rumex occidentalis</t>
+  </si>
+  <si>
+    <t>Western Trillium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trillium vatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Clematis </t>
+  </si>
+  <si>
+    <t>Clematis ligusticifolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood Groundsel </t>
+  </si>
+  <si>
+    <t>Senecio sylvaticus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yarrow </t>
+  </si>
+  <si>
+    <t>Achillea millefolium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARU </t>
+  </si>
+  <si>
+    <t>Cyspp</t>
+  </si>
+  <si>
+    <t>Laspp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA </t>
   </si>
 </sst>
 </file>
@@ -350,13 +1404,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -676,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2632A-81E2-4372-B21A-08C497B1BE35}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:E27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,16 +1742,16 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -708,7 +1762,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -719,7 +1773,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -730,7 +1784,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -741,19 +1795,19 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
@@ -761,7 +1815,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -778,7 +1832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -794,7 +1848,7 @@
       </c>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -812,7 +1866,7 @@
       </c>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
@@ -944,7 +1998,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -955,7 +2009,9 @@
       <c r="D20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -970,7 +2026,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -981,7 +2037,9 @@
       <c r="D22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -996,7 +2054,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>39</v>
       </c>
@@ -1007,7 +2065,9 @@
       <c r="D24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1058,4 +2118,2322 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7228CDBB-DB00-426D-AD0F-AFD6D1409B4C}">
+  <dimension ref="A1:G115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" t="s">
+        <v>412</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" t="s">
+        <v>219</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" t="s">
+        <v>232</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>238</v>
+      </c>
+      <c r="D26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>245</v>
+      </c>
+      <c r="D30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D31" t="s">
+        <v>248</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" t="s">
+        <v>250</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" t="s">
+        <v>252</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>253</v>
+      </c>
+      <c r="D34" t="s">
+        <v>254</v>
+      </c>
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" t="s">
+        <v>256</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>257</v>
+      </c>
+      <c r="D36" t="s">
+        <v>258</v>
+      </c>
+      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" t="s">
+        <v>260</v>
+      </c>
+      <c r="E37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E38" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>265</v>
+      </c>
+      <c r="D40" t="s">
+        <v>266</v>
+      </c>
+      <c r="E40" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>267</v>
+      </c>
+      <c r="D41" t="s">
+        <v>268</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>269</v>
+      </c>
+      <c r="D42" t="s">
+        <v>270</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
+        <v>271</v>
+      </c>
+      <c r="D43" t="s">
+        <v>272</v>
+      </c>
+      <c r="E43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>273</v>
+      </c>
+      <c r="D44" t="s">
+        <v>274</v>
+      </c>
+      <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
+        <v>275</v>
+      </c>
+      <c r="D45" t="s">
+        <v>276</v>
+      </c>
+      <c r="E45" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
+        <v>279</v>
+      </c>
+      <c r="D47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" t="s">
+        <v>281</v>
+      </c>
+      <c r="E48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" t="s">
+        <v>283</v>
+      </c>
+      <c r="E49" t="s">
+        <v>124</v>
+      </c>
+      <c r="F49" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" t="s">
+        <v>285</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50">
+        <v>5</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>286</v>
+      </c>
+      <c r="D51" t="s">
+        <v>287</v>
+      </c>
+      <c r="E51" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>288</v>
+      </c>
+      <c r="D52" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" t="s">
+        <v>127</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>291</v>
+      </c>
+      <c r="D53" t="s">
+        <v>292</v>
+      </c>
+      <c r="E53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" t="s">
+        <v>95</v>
+      </c>
+      <c r="G53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" t="s">
+        <v>293</v>
+      </c>
+      <c r="D54" t="s">
+        <v>294</v>
+      </c>
+      <c r="E54" t="s">
+        <v>129</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>295</v>
+      </c>
+      <c r="D55" t="s">
+        <v>296</v>
+      </c>
+      <c r="E55" t="s">
+        <v>130</v>
+      </c>
+      <c r="F55" t="s">
+        <v>95</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>297</v>
+      </c>
+      <c r="D56" t="s">
+        <v>298</v>
+      </c>
+      <c r="E56" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>299</v>
+      </c>
+      <c r="D57" t="s">
+        <v>300</v>
+      </c>
+      <c r="E57" t="s">
+        <v>132</v>
+      </c>
+      <c r="F57" t="s">
+        <v>95</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>301</v>
+      </c>
+      <c r="D58" t="s">
+        <v>302</v>
+      </c>
+      <c r="E58" t="s">
+        <v>133</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>303</v>
+      </c>
+      <c r="D59" t="s">
+        <v>304</v>
+      </c>
+      <c r="E59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>305</v>
+      </c>
+      <c r="D60" t="s">
+        <v>306</v>
+      </c>
+      <c r="E60" t="s">
+        <v>135</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" t="s">
+        <v>307</v>
+      </c>
+      <c r="D61" t="s">
+        <v>308</v>
+      </c>
+      <c r="E61" t="s">
+        <v>413</v>
+      </c>
+      <c r="F61">
+        <v>4</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" t="s">
+        <v>309</v>
+      </c>
+      <c r="D62" t="s">
+        <v>310</v>
+      </c>
+      <c r="E62" t="s">
+        <v>137</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" t="s">
+        <v>311</v>
+      </c>
+      <c r="D63" t="s">
+        <v>312</v>
+      </c>
+      <c r="E63" t="s">
+        <v>138</v>
+      </c>
+      <c r="F63" t="s">
+        <v>95</v>
+      </c>
+      <c r="G63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" t="s">
+        <v>313</v>
+      </c>
+      <c r="D64" t="s">
+        <v>314</v>
+      </c>
+      <c r="E64" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64" t="s">
+        <v>95</v>
+      </c>
+      <c r="G64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
+        <v>315</v>
+      </c>
+      <c r="D65" t="s">
+        <v>316</v>
+      </c>
+      <c r="E65" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65" t="s">
+        <v>95</v>
+      </c>
+      <c r="G65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>317</v>
+      </c>
+      <c r="D66" t="s">
+        <v>318</v>
+      </c>
+      <c r="E66" t="s">
+        <v>141</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>319</v>
+      </c>
+      <c r="D67" t="s">
+        <v>320</v>
+      </c>
+      <c r="E67" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67" t="s">
+        <v>95</v>
+      </c>
+      <c r="G67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" t="s">
+        <v>321</v>
+      </c>
+      <c r="D68" t="s">
+        <v>322</v>
+      </c>
+      <c r="E68" t="s">
+        <v>143</v>
+      </c>
+      <c r="F68" t="s">
+        <v>95</v>
+      </c>
+      <c r="G68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
+        <v>323</v>
+      </c>
+      <c r="D69" t="s">
+        <v>324</v>
+      </c>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
+      <c r="F69" t="s">
+        <v>95</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" t="s">
+        <v>325</v>
+      </c>
+      <c r="D70" t="s">
+        <v>326</v>
+      </c>
+      <c r="E70" t="s">
+        <v>145</v>
+      </c>
+      <c r="F70" t="s">
+        <v>95</v>
+      </c>
+      <c r="G70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" t="s">
+        <v>327</v>
+      </c>
+      <c r="D71" t="s">
+        <v>328</v>
+      </c>
+      <c r="E71" t="s">
+        <v>146</v>
+      </c>
+      <c r="F71" t="s">
+        <v>95</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" t="s">
+        <v>329</v>
+      </c>
+      <c r="D72" t="s">
+        <v>330</v>
+      </c>
+      <c r="E72" t="s">
+        <v>147</v>
+      </c>
+      <c r="F72" t="s">
+        <v>95</v>
+      </c>
+      <c r="G72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
+        <v>331</v>
+      </c>
+      <c r="D74" t="s">
+        <v>332</v>
+      </c>
+      <c r="E74" t="s">
+        <v>150</v>
+      </c>
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" t="s">
+        <v>333</v>
+      </c>
+      <c r="D75" t="s">
+        <v>334</v>
+      </c>
+      <c r="E75" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" t="s">
+        <v>95</v>
+      </c>
+      <c r="G75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" t="s">
+        <v>153</v>
+      </c>
+      <c r="F76">
+        <v>5</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" t="s">
+        <v>335</v>
+      </c>
+      <c r="D77" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" t="s">
+        <v>414</v>
+      </c>
+      <c r="F77" t="s">
+        <v>95</v>
+      </c>
+      <c r="G77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" t="s">
+        <v>336</v>
+      </c>
+      <c r="D78" t="s">
+        <v>337</v>
+      </c>
+      <c r="E78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F78" t="s">
+        <v>95</v>
+      </c>
+      <c r="G78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" t="s">
+        <v>338</v>
+      </c>
+      <c r="D79" t="s">
+        <v>339</v>
+      </c>
+      <c r="E79" t="s">
+        <v>156</v>
+      </c>
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>136</v>
+      </c>
+      <c r="C80" t="s">
+        <v>340</v>
+      </c>
+      <c r="D80" t="s">
+        <v>341</v>
+      </c>
+      <c r="E80" t="s">
+        <v>157</v>
+      </c>
+      <c r="F80" t="s">
+        <v>95</v>
+      </c>
+      <c r="G80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" t="s">
+        <v>342</v>
+      </c>
+      <c r="D81" t="s">
+        <v>343</v>
+      </c>
+      <c r="E81" t="s">
+        <v>158</v>
+      </c>
+      <c r="F81" t="s">
+        <v>95</v>
+      </c>
+      <c r="G81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" t="s">
+        <v>344</v>
+      </c>
+      <c r="D82" t="s">
+        <v>345</v>
+      </c>
+      <c r="E82" t="s">
+        <v>159</v>
+      </c>
+      <c r="F82">
+        <v>4</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C83" t="s">
+        <v>346</v>
+      </c>
+      <c r="D83" t="s">
+        <v>347</v>
+      </c>
+      <c r="E83" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83">
+        <v>4</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" t="s">
+        <v>348</v>
+      </c>
+      <c r="D84" t="s">
+        <v>349</v>
+      </c>
+      <c r="E84" t="s">
+        <v>161</v>
+      </c>
+      <c r="F84" t="s">
+        <v>95</v>
+      </c>
+      <c r="G84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" t="s">
+        <v>350</v>
+      </c>
+      <c r="D85" t="s">
+        <v>351</v>
+      </c>
+      <c r="E85" t="s">
+        <v>162</v>
+      </c>
+      <c r="F85" t="s">
+        <v>95</v>
+      </c>
+      <c r="G85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" t="s">
+        <v>352</v>
+      </c>
+      <c r="D86" t="s">
+        <v>353</v>
+      </c>
+      <c r="E86" t="s">
+        <v>163</v>
+      </c>
+      <c r="F86">
+        <v>6</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" t="s">
+        <v>354</v>
+      </c>
+      <c r="D87" t="s">
+        <v>355</v>
+      </c>
+      <c r="E87" t="s">
+        <v>415</v>
+      </c>
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" t="s">
+        <v>356</v>
+      </c>
+      <c r="D88" t="s">
+        <v>357</v>
+      </c>
+      <c r="E88" t="s">
+        <v>164</v>
+      </c>
+      <c r="F88">
+        <v>4</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>136</v>
+      </c>
+      <c r="C89" t="s">
+        <v>358</v>
+      </c>
+      <c r="D89" t="s">
+        <v>359</v>
+      </c>
+      <c r="E89" t="s">
+        <v>165</v>
+      </c>
+      <c r="F89" t="s">
+        <v>95</v>
+      </c>
+      <c r="G89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>136</v>
+      </c>
+      <c r="C90" t="s">
+        <v>360</v>
+      </c>
+      <c r="D90" t="s">
+        <v>361</v>
+      </c>
+      <c r="E90" t="s">
+        <v>166</v>
+      </c>
+      <c r="F90">
+        <v>5</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>136</v>
+      </c>
+      <c r="C91" t="s">
+        <v>362</v>
+      </c>
+      <c r="D91" t="s">
+        <v>363</v>
+      </c>
+      <c r="E91" t="s">
+        <v>167</v>
+      </c>
+      <c r="F91" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>136</v>
+      </c>
+      <c r="C92" t="s">
+        <v>364</v>
+      </c>
+      <c r="D92" t="s">
+        <v>365</v>
+      </c>
+      <c r="E92" t="s">
+        <v>168</v>
+      </c>
+      <c r="F92" t="s">
+        <v>95</v>
+      </c>
+      <c r="G92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>136</v>
+      </c>
+      <c r="C93" t="s">
+        <v>366</v>
+      </c>
+      <c r="D93" t="s">
+        <v>367</v>
+      </c>
+      <c r="E93" t="s">
+        <v>416</v>
+      </c>
+      <c r="F93">
+        <v>4</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>136</v>
+      </c>
+      <c r="C94" t="s">
+        <v>368</v>
+      </c>
+      <c r="D94" t="s">
+        <v>369</v>
+      </c>
+      <c r="E94" t="s">
+        <v>169</v>
+      </c>
+      <c r="F94" t="s">
+        <v>95</v>
+      </c>
+      <c r="G94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" t="s">
+        <v>370</v>
+      </c>
+      <c r="D95" t="s">
+        <v>371</v>
+      </c>
+      <c r="E95" t="s">
+        <v>417</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>136</v>
+      </c>
+      <c r="C96" t="s">
+        <v>372</v>
+      </c>
+      <c r="D96" t="s">
+        <v>373</v>
+      </c>
+      <c r="E96" t="s">
+        <v>170</v>
+      </c>
+      <c r="F96">
+        <v>6</v>
+      </c>
+      <c r="G96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C97" t="s">
+        <v>374</v>
+      </c>
+      <c r="D97" t="s">
+        <v>375</v>
+      </c>
+      <c r="E97" t="s">
+        <v>171</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>136</v>
+      </c>
+      <c r="C98" t="s">
+        <v>376</v>
+      </c>
+      <c r="D98" t="s">
+        <v>377</v>
+      </c>
+      <c r="E98" t="s">
+        <v>418</v>
+      </c>
+      <c r="F98" t="s">
+        <v>95</v>
+      </c>
+      <c r="G98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>136</v>
+      </c>
+      <c r="C99" t="s">
+        <v>378</v>
+      </c>
+      <c r="D99" t="s">
+        <v>379</v>
+      </c>
+      <c r="E99" t="s">
+        <v>172</v>
+      </c>
+      <c r="F99" t="s">
+        <v>95</v>
+      </c>
+      <c r="G99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>136</v>
+      </c>
+      <c r="C100" t="s">
+        <v>380</v>
+      </c>
+      <c r="D100" t="s">
+        <v>381</v>
+      </c>
+      <c r="E100" t="s">
+        <v>173</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" t="s">
+        <v>382</v>
+      </c>
+      <c r="D101" t="s">
+        <v>383</v>
+      </c>
+      <c r="E101" t="s">
+        <v>174</v>
+      </c>
+      <c r="F101">
+        <v>2</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" t="s">
+        <v>384</v>
+      </c>
+      <c r="D102" t="s">
+        <v>385</v>
+      </c>
+      <c r="E102" t="s">
+        <v>140</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+      <c r="G102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>136</v>
+      </c>
+      <c r="C103" t="s">
+        <v>386</v>
+      </c>
+      <c r="D103" t="s">
+        <v>387</v>
+      </c>
+      <c r="E103" t="s">
+        <v>175</v>
+      </c>
+      <c r="F103">
+        <v>4</v>
+      </c>
+      <c r="G103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>136</v>
+      </c>
+      <c r="C104" t="s">
+        <v>388</v>
+      </c>
+      <c r="D104" t="s">
+        <v>389</v>
+      </c>
+      <c r="E104" t="s">
+        <v>176</v>
+      </c>
+      <c r="F104">
+        <v>6</v>
+      </c>
+      <c r="G104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>136</v>
+      </c>
+      <c r="C105" t="s">
+        <v>390</v>
+      </c>
+      <c r="D105" t="s">
+        <v>391</v>
+      </c>
+      <c r="E105" t="s">
+        <v>419</v>
+      </c>
+      <c r="F105">
+        <v>6</v>
+      </c>
+      <c r="G105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>136</v>
+      </c>
+      <c r="C106" t="s">
+        <v>392</v>
+      </c>
+      <c r="D106" t="s">
+        <v>393</v>
+      </c>
+      <c r="E106" t="s">
+        <v>177</v>
+      </c>
+      <c r="F106">
+        <v>4</v>
+      </c>
+      <c r="G106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>136</v>
+      </c>
+      <c r="C107" t="s">
+        <v>394</v>
+      </c>
+      <c r="D107" t="s">
+        <v>395</v>
+      </c>
+      <c r="E107" t="s">
+        <v>178</v>
+      </c>
+      <c r="F107">
+        <v>4</v>
+      </c>
+      <c r="G107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" t="s">
+        <v>396</v>
+      </c>
+      <c r="D108" t="s">
+        <v>397</v>
+      </c>
+      <c r="E108" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" t="s">
+        <v>95</v>
+      </c>
+      <c r="G108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>136</v>
+      </c>
+      <c r="C109" t="s">
+        <v>398</v>
+      </c>
+      <c r="D109" t="s">
+        <v>399</v>
+      </c>
+      <c r="E109" t="s">
+        <v>180</v>
+      </c>
+      <c r="F109">
+        <v>4</v>
+      </c>
+      <c r="G109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>136</v>
+      </c>
+      <c r="C110" t="s">
+        <v>400</v>
+      </c>
+      <c r="D110" t="s">
+        <v>401</v>
+      </c>
+      <c r="E110" t="s">
+        <v>181</v>
+      </c>
+      <c r="F110" t="s">
+        <v>95</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>136</v>
+      </c>
+      <c r="C111" t="s">
+        <v>402</v>
+      </c>
+      <c r="D111" t="s">
+        <v>403</v>
+      </c>
+      <c r="E111" t="s">
+        <v>182</v>
+      </c>
+      <c r="F111" t="s">
+        <v>95</v>
+      </c>
+      <c r="G111" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>136</v>
+      </c>
+      <c r="C112" t="s">
+        <v>404</v>
+      </c>
+      <c r="D112" t="s">
+        <v>405</v>
+      </c>
+      <c r="E112" t="s">
+        <v>183</v>
+      </c>
+      <c r="F112">
+        <v>4</v>
+      </c>
+      <c r="G112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>136</v>
+      </c>
+      <c r="C113" t="s">
+        <v>406</v>
+      </c>
+      <c r="D113" t="s">
+        <v>407</v>
+      </c>
+      <c r="E113" t="s">
+        <v>184</v>
+      </c>
+      <c r="F113" t="s">
+        <v>95</v>
+      </c>
+      <c r="G113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>136</v>
+      </c>
+      <c r="C114" t="s">
+        <v>408</v>
+      </c>
+      <c r="D114" t="s">
+        <v>409</v>
+      </c>
+      <c r="E114" t="s">
+        <v>185</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" t="s">
+        <v>410</v>
+      </c>
+      <c r="D115" t="s">
+        <v>411</v>
+      </c>
+      <c r="E115" t="s">
+        <v>77</v>
+      </c>
+      <c r="F115">
+        <v>2</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:G1" xr:uid="{11646EBE-9FA0-4AB4-A4FE-DF425FCE2B01}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>